<commit_message>
ACTIVIDAD ULTIMAS FOTOS COONFIGURACION DE PATRON VIEW HOLDER
</commit_message>
<xml_diff>
--- a/Analisis.xlsx
+++ b/Analisis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16035" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Botones Activ Principal" sheetId="2" r:id="rId3"/>
     <sheet name="Diagrama Flujo Activ Principal" sheetId="1" r:id="rId4"/>
     <sheet name="Botones Activ Analizar" sheetId="4" r:id="rId5"/>
-    <sheet name="Diagrama Flujo Activ Analizar" sheetId="3" r:id="rId6"/>
+    <sheet name="Botones Activ Ultimas Fotos" sheetId="7" r:id="rId6"/>
+    <sheet name="Diagrama Flujo Activ Analizar" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -8537,7 +8538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -8567,7 +8568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -8582,6 +8583,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>

</xml_diff>